<commit_message>
Added new experiment input for WiFi anomaly
</commit_message>
<xml_diff>
--- a/input/Final Design- 2000 runs 1a.xlsx
+++ b/input/Final Design- 2000 runs 1a.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melissa.n.jablonski\Documents\Liza Drone Swarm Research\20210408_QoK_r1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ross.arnold\Documents\Work\Projects\SNA ILIR\dronelab\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -386,7 +386,7 @@
   <dimension ref="A1:F501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,22 +419,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3.1053451980055824E-2</v>
+        <v>1.7732689181804151E-2</v>
       </c>
       <c r="B2">
-        <v>0.43855014426719219</v>
+        <v>0.2398547486262026</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>